<commit_message>
restructuring + final change
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheMonke\Documents\Desktop\MA\Jaar3\DTT_Maze_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1BA70-F449-4DAA-A166-B79977DB75CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0371D0C4-1356-48AB-AC55-CF71AC56191A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1924,7 +1924,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>